<commit_message>
Updated DD2090 docs and CAD files.
</commit_message>
<xml_diff>
--- a/DD2090FFC_DepthAI_4-camera_FFC/Docs/Assembly Outputs/BOM/BOM-DD2090_4CAM_FFC_ACTIVE_BOM(Production).xlsx
+++ b/DD2090FFC_DepthAI_4-camera_FFC/Docs/Assembly Outputs/BOM/BOM-DD2090_4CAM_FFC_ACTIVE_BOM(Production).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="215">
   <si>
     <t>Name</t>
   </si>
@@ -66,96 +66,135 @@
     <t>DTSM-32N-V</t>
   </si>
   <si>
+    <t>2.2uF 0402</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>CAP CER 2.2UF 10V X5R 0402 10%</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>GRM155R61A225KE95D</t>
+  </si>
+  <si>
+    <t>CAPC0402(1005)70_L</t>
+  </si>
+  <si>
+    <t>22uF 0603</t>
+  </si>
+  <si>
+    <t>C2, C3, C4, C13, C14, C15, C16</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 10V X5R 0603 20%</t>
+  </si>
+  <si>
+    <t>GRM188R61A226ME15D</t>
+  </si>
+  <si>
+    <t>CAPC0603(1608)100_L, CAPC0603(1608)100_N</t>
+  </si>
+  <si>
+    <t>1uF 0402</t>
+  </si>
+  <si>
+    <t>C5, C8</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 25V X5R 0402 10%</t>
+  </si>
+  <si>
+    <t>GRM155R61E105KA12D</t>
+  </si>
+  <si>
+    <t>CAPC0402(1005)70_N</t>
+  </si>
+  <si>
     <t>10uF 0603</t>
   </si>
   <si>
-    <t>C1, C6, C7, C42, C43</t>
+    <t>C6, C7, C42, C43</t>
   </si>
   <si>
     <t>CAP CER 10UF 10V X5R 0603 20%</t>
   </si>
   <si>
-    <t>Murata</t>
-  </si>
-  <si>
     <t>GRM188R61A106ME69D</t>
   </si>
   <si>
     <t>CAPC0603(1608)100_L</t>
   </si>
   <si>
-    <t>22uF 0603</t>
-  </si>
-  <si>
-    <t>C2, C3, C4</t>
-  </si>
-  <si>
-    <t>CAP CER 22UF 10V X5R 0603 20%</t>
-  </si>
-  <si>
-    <t>GRM188R61A226ME15D</t>
+    <t>0.1uF 0402</t>
+  </si>
+  <si>
+    <t>C9, C10, C44, C45, C46</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 10V X7R 0402 5%</t>
+  </si>
+  <si>
+    <t>GRM155R71A104JA01D</t>
+  </si>
+  <si>
+    <t>0.1uF 0201</t>
+  </si>
+  <si>
+    <t>C11, C12, C208, C209, C211, C212</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 10V X5R 0201</t>
+  </si>
+  <si>
+    <t>GRM033R61A104KE15D</t>
+  </si>
+  <si>
+    <t>CAPC0201(0603)33_L</t>
+  </si>
+  <si>
+    <t>33pF 0201</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>CAP CER 33PF 25V C0G/NP0 0201</t>
+  </si>
+  <si>
+    <t>GRM0335C1E330JA01D</t>
+  </si>
+  <si>
+    <t>18pF 0201</t>
+  </si>
+  <si>
+    <t>C47, C48</t>
+  </si>
+  <si>
+    <t>Cap Ceramic 18pF 25V C0G 1% Pad SMD 0201 125C T/R</t>
+  </si>
+  <si>
+    <t>GRM0335C1E180FA01D</t>
+  </si>
+  <si>
+    <t>4.7uF 0603</t>
+  </si>
+  <si>
+    <t>C55</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 16V X5R 0603 10%</t>
+  </si>
+  <si>
+    <t>GRM188R61C475KAAJD</t>
   </si>
   <si>
     <t>CAPC0603(1608)100_N</t>
   </si>
   <si>
-    <t>1uF 0402</t>
-  </si>
-  <si>
-    <t>C5, C8</t>
-  </si>
-  <si>
-    <t>CAP CER 1UF 25V X5R 0402 10%</t>
-  </si>
-  <si>
-    <t>GRM155R61E105KA12D</t>
-  </si>
-  <si>
-    <t>CAPC0402(1005)70_N</t>
-  </si>
-  <si>
-    <t>0.1uF 0402</t>
-  </si>
-  <si>
-    <t>C9, C10, C44, C45, C46</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 10V X7R 0402 5%</t>
-  </si>
-  <si>
-    <t>GRM155R71A104JA01D</t>
-  </si>
-  <si>
-    <t>CAPC0402(1005)70_L</t>
-  </si>
-  <si>
-    <t>18pF 0201</t>
-  </si>
-  <si>
-    <t>C47, C48</t>
-  </si>
-  <si>
-    <t>Cap Ceramic 18pF 25V C0G 1% Pad SMD 0201 125C T/R</t>
-  </si>
-  <si>
-    <t>GRM0335C1E180FA01D</t>
-  </si>
-  <si>
-    <t>CAPC0201(0603)33_L</t>
-  </si>
-  <si>
-    <t>4.7uF 0603</t>
-  </si>
-  <si>
-    <t>C55</t>
-  </si>
-  <si>
-    <t>CAP CER 4.7UF 16V X5R 0603 10%</t>
-  </si>
-  <si>
-    <t>GRM188R61C475KAAJD</t>
-  </si>
-  <si>
     <t>10uF 0402</t>
   </si>
   <si>
@@ -168,18 +207,6 @@
     <t>GRM155R60J106ME15D</t>
   </si>
   <si>
-    <t>0.1uF 0201</t>
-  </si>
-  <si>
-    <t>C208, C209, C211, C212</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 10V X5R 0201</t>
-  </si>
-  <si>
-    <t>GRM033R61A104KE15D</t>
-  </si>
-  <si>
     <t>RED 0603</t>
   </si>
   <si>
@@ -435,33 +462,33 @@
     <t>RESC0603(1608)_N, RESC0603(1608)_L</t>
   </si>
   <si>
-    <t>97.6K 0402</t>
+    <t>90.9K 0402</t>
   </si>
   <si>
     <t>R8</t>
   </si>
   <si>
-    <t>RES SMD 97.6K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>CRCW040297K6FKED</t>
+    <t>RES SMD 90.9K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>CRCW040290K9FKED</t>
+  </si>
+  <si>
+    <t>22R 0402</t>
+  </si>
+  <si>
+    <t>R10, R12</t>
+  </si>
+  <si>
+    <t>RES SMD 22 OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RC0402FR-0722RL</t>
   </si>
   <si>
     <t>RESC0402(1005)_N</t>
   </si>
   <si>
-    <t>22R 0402</t>
-  </si>
-  <si>
-    <t>R10, R12</t>
-  </si>
-  <si>
-    <t>RES SMD 22 OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>RC0402FR-0722RL</t>
-  </si>
-  <si>
     <t>10K 0402</t>
   </si>
   <si>
@@ -477,16 +504,16 @@
     <t>RESC0402(1005)_L, RESC0402(1005)_N</t>
   </si>
   <si>
-    <t>442K 0402</t>
+    <t>20K 0402</t>
   </si>
   <si>
     <t>R25</t>
   </si>
   <si>
-    <t>RES SMD 442K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>CRCW0402442KFKED</t>
+    <t>RES SMD 20K OHM 1% 1/16W 0402 20 kOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film</t>
+  </si>
+  <si>
+    <t>RC0402FR-0720KL</t>
   </si>
   <si>
     <t>0R 0402</t>
@@ -513,13 +540,19 @@
     <t>CRCW04021M80FKED</t>
   </si>
   <si>
-    <t>TLV62568DRLR</t>
+    <t>TPS51313DRCR</t>
   </si>
   <si>
     <t>U1</t>
   </si>
   <si>
-    <t>IC REG BUCK ADJ 1A SOT563-6</t>
+    <t>Switching Regulator, Voltage-mode, 3A, 1000kHz Switching Freq-Max, PDSO10</t>
+  </si>
+  <si>
+    <t>TPS51313DRCT</t>
+  </si>
+  <si>
+    <t>VSON-TPS51313DRCR</t>
   </si>
   <si>
     <t>1.5A ideal diode</t>
@@ -594,10 +627,16 @@
     <t>U61</t>
   </si>
   <si>
-    <t>IC MUX 2:1 8 OHM 20VQFN</t>
-  </si>
-  <si>
-    <t>HD3SS3212RKSR</t>
+    <t>Multiplexer And Demux/Decoder, CBT/FST/QS/5C/B Series, 1-Func, 2 Line Input, 1 Line Output, True Output, PQCC20</t>
+  </si>
+  <si>
+    <t>NXP Semiconductors</t>
+  </si>
+  <si>
+    <t>CBTL02043ABQ,115</t>
+  </si>
+  <si>
+    <t>CBTL02043A</t>
   </si>
   <si>
     <t>USB Type-C Port Control</t>
@@ -899,7 +938,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
@@ -980,7 +1019,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>17</v>
@@ -1009,7 +1048,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>23</v>
@@ -1067,7 +1106,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>33</v>
@@ -1096,7 +1135,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>38</v>
@@ -1111,7 +1150,7 @@
         <v>40</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>40</v>
@@ -1122,31 +1161,31 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="17">
+        <v>6</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="17">
-        <v>1</v>
-      </c>
-      <c r="C8" s="16" t="s">
+      <c r="D8" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>44</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>26</v>
-      </c>
       <c r="H8" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1154,7 +1193,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>47</v>
@@ -1169,7 +1208,7 @@
         <v>49</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>49</v>
@@ -1183,7 +1222,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>51</v>
@@ -1198,7 +1237,7 @@
         <v>53</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>53</v>
@@ -1221,77 +1260,77 @@
         <v>56</v>
       </c>
       <c r="E11" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="G11" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>59</v>
-      </c>
       <c r="H11" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="17">
+        <v>4</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="17">
-        <v>2</v>
-      </c>
-      <c r="C12" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="E12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>63</v>
-      </c>
       <c r="G12" s="16" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="17">
         <v>1</v>
       </c>
       <c r="C13" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>67</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>68</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>68</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1299,7 +1338,7 @@
         <v>69</v>
       </c>
       <c r="B14" s="17">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>70</v>
@@ -1308,19 +1347,19 @@
         <v>71</v>
       </c>
       <c r="E14" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>69</v>
-      </c>
       <c r="G14" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1328,7 +1367,7 @@
         <v>73</v>
       </c>
       <c r="B15" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>74</v>
@@ -1343,175 +1382,175 @@
         <v>77</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="17">
+        <v>13</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="17">
-        <v>1</v>
-      </c>
-      <c r="C16" s="16" t="s">
+      <c r="E16" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>83</v>
-      </c>
       <c r="F16" s="16" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="17">
-        <v>4</v>
-      </c>
-      <c r="C17" s="16" t="s">
+      <c r="G17" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="H17" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>90</v>
-      </c>
       <c r="I17" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B18" s="17">
         <v>1</v>
       </c>
       <c r="C18" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="F18" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="G18" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>95</v>
-      </c>
       <c r="H18" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="17">
+        <v>4</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="17">
-        <v>1</v>
-      </c>
-      <c r="C19" s="16" t="s">
+      <c r="D19" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="F19" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>100</v>
-      </c>
       <c r="G19" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="17">
         <v>1</v>
       </c>
       <c r="C20" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="E20" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="F20" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>105</v>
-      </c>
       <c r="G20" s="16" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="17">
         <v>1</v>
       </c>
       <c r="C21" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="E21" s="16" t="s">
         <v>108</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>94</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>109</v>
@@ -1540,222 +1579,222 @@
         <v>112</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B23" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="28" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B24" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B25" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>126</v>
-      </c>
       <c r="G25" s="16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="17">
+        <v>2</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="17">
-        <v>8</v>
-      </c>
-      <c r="C26" s="16" t="s">
+      <c r="E26" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="F26" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>131</v>
-      </c>
       <c r="G26" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="17">
+        <v>2</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="17">
-        <v>7</v>
-      </c>
-      <c r="C27" s="16" t="s">
+      <c r="E27" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="F27" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="G27" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="F27" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>138</v>
-      </c>
       <c r="H27" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="17">
+        <v>8</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B28" s="17">
-        <v>1</v>
-      </c>
-      <c r="C28" s="16" t="s">
+      <c r="E28" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="F28" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="G28" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>143</v>
-      </c>
       <c r="H28" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="17">
+        <v>7</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="17">
-        <v>2</v>
-      </c>
-      <c r="C29" s="16" t="s">
+      <c r="E29" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="F29" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="16" t="s">
+      <c r="G29" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="G29" s="16" t="s">
-        <v>143</v>
-      </c>
       <c r="H29" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1763,7 +1802,7 @@
         <v>148</v>
       </c>
       <c r="B30" s="17">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>149</v>
@@ -1772,13 +1811,13 @@
         <v>150</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="F30" s="16" t="s">
         <v>151</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="H30" s="16" t="s">
         <v>151</v>
@@ -1789,31 +1828,31 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B31" s="17">
+        <v>2</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="B31" s="17">
-        <v>1</v>
-      </c>
-      <c r="C31" s="16" t="s">
+      <c r="D31" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="E31" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="F31" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="E31" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" s="16" t="s">
+      <c r="G31" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="G31" s="16" t="s">
-        <v>143</v>
-      </c>
       <c r="H31" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1821,7 +1860,7 @@
         <v>157</v>
       </c>
       <c r="B32" s="17">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>158</v>
@@ -1830,13 +1869,13 @@
         <v>159</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F32" s="16" t="s">
         <v>160</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="H32" s="16" t="s">
         <v>160</v>
@@ -1847,251 +1886,251 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="28" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B33" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E33" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="G33" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="F33" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>143</v>
-      </c>
       <c r="H33" s="16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B34" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="28" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B35" s="17">
         <v>2</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="28" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B36" s="17">
         <v>1</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D36" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="H36" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="E36" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>172</v>
-      </c>
       <c r="I36" s="16" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="28" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B37" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>179</v>
+        <v>81</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="28" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B38" s="17">
         <v>1</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D38" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="G38" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="E38" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>185</v>
-      </c>
       <c r="H38" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B39" s="17">
         <v>1</v>
       </c>
       <c r="C39" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="F39" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="D39" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>186</v>
-      </c>
       <c r="G39" s="16" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="28" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B40" s="17">
         <v>1</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>72</v>
+        <v>195</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="28" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B41" s="17">
         <v>1</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>72</v>
+        <v>200</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>197</v>
@@ -2108,31 +2147,89 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="28" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B42" s="17">
         <v>1</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>198</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" s="17">
+        <v>1</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="I43" s="16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="B44" s="17">
+        <v>1</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="I44" s="16" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated design and production files Image photos and other files to be updated
</commit_message>
<xml_diff>
--- a/DD2090FFC_DepthAI_4-camera_FFC/Docs/Assembly Outputs/BOM/BOM-DD2090_4CAM_FFC_ACTIVE_BOM(Production).xlsx
+++ b/DD2090FFC_DepthAI_4-camera_FFC/Docs/Assembly Outputs/BOM/BOM-DD2090_4CAM_FFC_ACTIVE_BOM(Production).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="204">
   <si>
     <t>Name</t>
   </si>
@@ -117,7 +117,7 @@
     <t>10uF 0603</t>
   </si>
   <si>
-    <t>C6, C7, C42, C43</t>
+    <t>C6, C7</t>
   </si>
   <si>
     <t>CAP CER 10UF 10V X5R 0603 20%</t>
@@ -132,7 +132,7 @@
     <t>0.1uF 0402</t>
   </si>
   <si>
-    <t>C9, C10, C44, C45, C46</t>
+    <t>C9, C10, C18, C19</t>
   </si>
   <si>
     <t>CAP CER 0.1UF 10V X7R 0402 5%</t>
@@ -168,18 +168,6 @@
     <t>GRM0335C1E330JA01D</t>
   </si>
   <si>
-    <t>18pF 0201</t>
-  </si>
-  <si>
-    <t>C47, C48</t>
-  </si>
-  <si>
-    <t>Cap Ceramic 18pF 25V C0G 1% Pad SMD 0201 125C T/R</t>
-  </si>
-  <si>
-    <t>GRM0335C1E180FA01D</t>
-  </si>
-  <si>
     <t>4.7uF 0603</t>
   </si>
   <si>
@@ -411,69 +399,57 @@
     <t>9774030243R</t>
   </si>
   <si>
-    <t>2.2K 0402</t>
-  </si>
-  <si>
-    <t>R1, R5</t>
-  </si>
-  <si>
-    <t>RES SMD 2.2K OHM 1% 1/16W 0402</t>
+    <t>1K 0402</t>
+  </si>
+  <si>
+    <t>R3, R4, R7, R15, R16, R26, R30, R61</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/16W 0402 1 kOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film, RES SMD 1K OHM 1% 1/16W 0402</t>
   </si>
   <si>
     <t>Yageo</t>
   </si>
   <si>
-    <t>RC0402FR-072K2L</t>
+    <t>RC0402FR-071KL</t>
+  </si>
+  <si>
+    <t>RESC0402(1005)_N, RESC0402(1005)_L</t>
+  </si>
+  <si>
+    <t>0R 0603</t>
+  </si>
+  <si>
+    <t>R6, R13, R14, R17, R18, R27, R36</t>
+  </si>
+  <si>
+    <t>RES SMD 0 OHM JUMPER 1/10W 0603 0 Ohms Jumper 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>CRCW06030000Z0EA</t>
+  </si>
+  <si>
+    <t>RESC0603(1608)_N, RESC0603(1608)_L</t>
+  </si>
+  <si>
+    <t>90.9K 0402</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>RES SMD 90.9K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>CRCW040290K9FKED</t>
   </si>
   <si>
     <t>RESC0402(1005)_L</t>
   </si>
   <si>
-    <t>1K 0402</t>
-  </si>
-  <si>
-    <t>R3, R4, R7, R15, R16, R26, R30, R61</t>
-  </si>
-  <si>
-    <t>RES SMD 1K OHM 1% 1/16W 0402 1 kOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film, RES SMD 1K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>RC0402FR-071KL</t>
-  </si>
-  <si>
-    <t>RESC0402(1005)_N, RESC0402(1005)_L</t>
-  </si>
-  <si>
-    <t>0R 0603</t>
-  </si>
-  <si>
-    <t>R6, R13, R14, R17, R18, R27, R36</t>
-  </si>
-  <si>
-    <t>RES SMD 0 OHM JUMPER 1/10W 0603 0 Ohms Jumper 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
-  </si>
-  <si>
-    <t>Vishay</t>
-  </si>
-  <si>
-    <t>CRCW06030000Z0EA</t>
-  </si>
-  <si>
-    <t>RESC0603(1608)_N, RESC0603(1608)_L</t>
-  </si>
-  <si>
-    <t>90.9K 0402</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>RES SMD 90.9K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>CRCW040290K9FKED</t>
-  </si>
-  <si>
     <t>22R 0402</t>
   </si>
   <si>
@@ -609,16 +585,19 @@
     <t>24AA32A-I/MS</t>
   </si>
   <si>
-    <t>BNO085</t>
-  </si>
-  <si>
-    <t>U12</t>
-  </si>
-  <si>
-    <t>IMU ACCEL/GYRO/MAG I2C 32BIT</t>
-  </si>
-  <si>
-    <t>CEVA</t>
+    <t>BMI270</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>Accelerometer, Gyroscope, 6 Axis Sensor IÂ²C, SPI Output</t>
+  </si>
+  <si>
+    <t>Bosch Sensortec</t>
+  </si>
+  <si>
+    <t>XDCR_BMI270</t>
   </si>
   <si>
     <t>USB Type-C Switch</t>
@@ -649,18 +628,6 @@
   </si>
   <si>
     <t>TUSB321RWBR</t>
-  </si>
-  <si>
-    <t>ABS06-127-32.768KHZ-T</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>CRYSTAL 32.768kHz ±20ppm Crystal 12.5pF 90 kOhms 2-SMD, No Lead</t>
-  </si>
-  <si>
-    <t>Abracon</t>
   </si>
 </sst>
 </file>
@@ -938,7 +905,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
@@ -1106,7 +1073,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>33</v>
@@ -1135,7 +1102,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>38</v>
@@ -1222,7 +1189,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>51</v>
@@ -1237,7 +1204,7 @@
         <v>53</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>53</v>
@@ -1248,31 +1215,31 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B11" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="16" t="s">
-        <v>57</v>
-      </c>
       <c r="I11" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1280,7 +1247,7 @@
         <v>59</v>
       </c>
       <c r="B12" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>60</v>
@@ -1289,48 +1256,48 @@
         <v>61</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="28" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B13" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="16" t="s">
+      <c r="H13" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="16" t="s">
-        <v>67</v>
-      </c>
       <c r="I13" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1338,7 +1305,7 @@
         <v>69</v>
       </c>
       <c r="B14" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>70</v>
@@ -1347,48 +1314,48 @@
         <v>71</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B15" s="17">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C15" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>77</v>
-      </c>
       <c r="G15" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1396,7 +1363,7 @@
         <v>78</v>
       </c>
       <c r="B16" s="17">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>79</v>
@@ -1408,184 +1375,184 @@
         <v>81</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="28" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B17" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="28" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B18" s="17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B19" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B20" s="17">
         <v>1</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B21" s="17">
         <v>1</v>
       </c>
       <c r="C21" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>109</v>
-      </c>
       <c r="H21" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B22" s="17">
         <v>1</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>114</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>114</v>
@@ -1608,7 +1575,7 @@
         <v>117</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>103</v>
+        <v>19</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>118</v>
@@ -1628,7 +1595,7 @@
         <v>119</v>
       </c>
       <c r="B24" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>120</v>
@@ -1637,251 +1604,251 @@
         <v>121</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="17">
+        <v>2</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B25" s="17">
-        <v>3</v>
-      </c>
-      <c r="C25" s="16" t="s">
+      <c r="D25" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="E25" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="16" t="s">
-        <v>66</v>
-      </c>
       <c r="F25" s="16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B26" s="17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="28" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B27" s="17">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="28" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B28" s="17">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="28" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B29" s="17">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G29" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="H29" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="H29" s="16" t="s">
-        <v>146</v>
-      </c>
       <c r="I29" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="28" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B30" s="17">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="28" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B31" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="28" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B32" s="17">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G32" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="H32" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="H32" s="16" t="s">
-        <v>160</v>
-      </c>
       <c r="I32" s="16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1889,7 +1856,7 @@
         <v>162</v>
       </c>
       <c r="B33" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>163</v>
@@ -1898,13 +1865,13 @@
         <v>164</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>165</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="H33" s="16" t="s">
         <v>165</v>
@@ -1918,7 +1885,7 @@
         <v>166</v>
       </c>
       <c r="B34" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>167</v>
@@ -1927,77 +1894,77 @@
         <v>168</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
       <c r="F34" s="16" t="s">
         <v>169</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="28" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B35" s="17">
         <v>2</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="28" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B36" s="17">
         <v>1</v>
       </c>
       <c r="C36" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="G36" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="D36" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>178</v>
-      </c>
       <c r="H36" s="16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2005,7 +1972,7 @@
         <v>179</v>
       </c>
       <c r="B37" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>180</v>
@@ -2014,222 +1981,135 @@
         <v>181</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>81</v>
+        <v>182</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="28" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B38" s="17">
         <v>1</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B39" s="17">
         <v>1</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D39" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="F39" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="E39" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>187</v>
-      </c>
       <c r="G39" s="16" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="28" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B40" s="17">
         <v>1</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="28" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B41" s="17">
         <v>1</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>200</v>
+        <v>77</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="B42" s="17">
-        <v>1</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="D42" s="16" t="s">
         <v>203</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="I42" s="16" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="B43" s="17">
-        <v>1</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="I43" s="16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="B44" s="17">
-        <v>1</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="I44" s="16" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>